<commit_message>
Started using express router, added api for adding new user,getting user,updating users array of books
</commit_message>
<xml_diff>
--- a/public/uploadedFile.xlsx
+++ b/public/uploadedFile.xlsx
@@ -62,11 +62,7 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>
-              Tarik 
-              <text:s/>
-              besic
-            </text:p>
+            <text:p>zijad zijic</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>
@@ -326,9 +322,9 @@
   <office:meta>
     <meta:creation-date>2017-10-20T23:41:04.964000000</meta:creation-date>
     <meta:generator>LibreOffice/7.0.6.2$Windows_X86_64 LibreOffice_project/144abb84a525d8e30c9dbbefa69cbbf2d8d4ae3b</meta:generator>
-    <dc:date>2021-09-01T15:39:33.457000000</dc:date>
-    <meta:editing-duration>PT37M9S</meta:editing-duration>
-    <meta:editing-cycles>17</meta:editing-cycles>
+    <dc:date>2021-09-04T00:25:00.271000000</dc:date>
+    <meta:editing-duration>PT37M23S</meta:editing-duration>
+    <meta:editing-cycles>18</meta:editing-cycles>
     <meta:document-statistic meta:table-count="1" meta:cell-count="49" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
@@ -347,8 +343,8 @@
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
-              <config:config-item config:name="CursorPositionX" config:type="int">1</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">16</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">3</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -573,9 +569,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2021-09-01">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2021-09-04">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="15:38:17.498000000">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="00:24:46.640000000">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>

<commit_message>
Added addClassController.js and booksController.js, added functionality to make rejected users table row red color
</commit_message>
<xml_diff>
--- a/public/uploadedFile.xlsx
+++ b/public/uploadedFile.xlsx
@@ -54,71 +54,41 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>test1 test1</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>test2 test2</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>test3 test3</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>test4 test4</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>test5 test5</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>tarik besic</text:p>
           </table:table-cell>
           <table:table-cell/>
         </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>zijad zijic</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>
-              ensar 
-              <text:s/>
-              dzafo
-            </text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>
-              amar 
-              <text:s text:c="12"/>
-              silajdzic
-            </text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>
-              benjamin 
-              <text:s text:c="12"/>
-              salkic
-            </text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>abbas merdan</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>evvel kamenjas</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>hamza kamenjas</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>neko nekic</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1" table:number-rows-repeated="5">
+        <table:table-row table:style-name="ro1" table:number-rows-repeated="8">
           <table:table-cell table:number-columns-repeated="2"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
@@ -129,7 +99,37 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>lamija besic</text:p>
+            <text:p>ciko cikic</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>cikone cikone</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>caklone caklone</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>cako2 cako2</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>cako3 cako3</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>cako4 cako4</text:p>
           </table:table-cell>
           <table:table-cell/>
         </table:table-row>
@@ -139,55 +139,7 @@
           </table:table-cell>
           <table:table-cell/>
         </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>fadil masnopita</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>edis musanovic</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>zijad mehic</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>emin bucuk</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>emin keskic</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>adnan abdukic</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>adnan hadzic</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>amar hamzic</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1" table:number-rows-repeated="11">
+        <table:table-row table:style-name="ro1" table:number-rows-repeated="14">
           <table:table-cell table:number-columns-repeated="2"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
@@ -198,25 +150,37 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>friyer1 frizer 2</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>friyzer2 frizer 2</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>frizer3 frizer 3</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>frizer4 frizer4</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>frizer5 frizer5</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>malena iki</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>haris hadzic</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>amra amric</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>anesa anesic</text:p>
           </table:table-cell>
           <table:table-cell/>
         </table:table-row>
@@ -232,10 +196,10 @@
   <office:meta>
     <meta:creation-date>2017-10-20T23:41:04.964000000</meta:creation-date>
     <meta:generator>LibreOffice/7.0.6.2$Windows_X86_64 LibreOffice_project/144abb84a525d8e30c9dbbefa69cbbf2d8d4ae3b</meta:generator>
-    <dc:date>2021-09-04T20:41:40.241000000</dc:date>
-    <meta:editing-duration>PT40M37S</meta:editing-duration>
-    <meta:editing-cycles>22</meta:editing-cycles>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="26" meta:object-count="0"/>
+    <dc:date>2021-09-16T20:12:58.243000000</dc:date>
+    <meta:editing-duration>PT43M4S</meta:editing-duration>
+    <meta:editing-cycles>24</meta:editing-cycles>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="22" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -247,14 +211,14 @@
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaWidth" config:type="int">5445</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">18965</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">19868</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
               <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">2</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">43</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -479,9 +443,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2021-09-04">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2021-09-16">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="20:41:28.291000000">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="20:12:43.014000000">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>

<commit_message>
Trimming values when adding Book
</commit_message>
<xml_diff>
--- a/public/uploadedFile.xlsx
+++ b/public/uploadedFile.xlsx
@@ -54,41 +54,71 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>test1 test1</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>test2 test2</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>test3 test3</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>test4 test4</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>test5 test5</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>tarik besic</text:p>
           </table:table-cell>
           <table:table-cell/>
         </table:table-row>
-        <table:table-row table:style-name="ro1" table:number-rows-repeated="8">
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>zijad zijic</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              ensar 
+              <text:s/>
+              dzafo
+            </text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              amar 
+              <text:s text:c="12"/>
+              silajdzic
+            </text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              benjamin 
+              <text:s text:c="12"/>
+              salkic
+            </text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>abbas merdan</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>evvel kamenjas</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>hamza kamenjas</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>neko nekic</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1" table:number-rows-repeated="5">
           <table:table-cell table:number-columns-repeated="2"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
@@ -99,37 +129,7 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>ciko cikic</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>cikone cikone</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>caklone caklone</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>cako2 cako2</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>cako3 cako3</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>cako4 cako4</text:p>
+            <text:p>lamija besic</text:p>
           </table:table-cell>
           <table:table-cell/>
         </table:table-row>
@@ -139,7 +139,55 @@
           </table:table-cell>
           <table:table-cell/>
         </table:table-row>
-        <table:table-row table:style-name="ro1" table:number-rows-repeated="14">
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>fadil masnopita</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>edis musanovic</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>zijad mehic</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>emin bucuk</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>emin keskic</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>adnan abdukic</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>adnan hadzic</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>amar hamzic</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1" table:number-rows-repeated="11">
           <table:table-cell table:number-columns-repeated="2"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
@@ -150,37 +198,25 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>friyer1 frizer 2</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>friyzer2 frizer 2</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>frizer3 frizer 3</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>frizer4 frizer4</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>frizer5 frizer5</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>malena iki</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>haris hadzic</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>amra amric</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>anesa anesic</text:p>
           </table:table-cell>
           <table:table-cell/>
         </table:table-row>
@@ -196,10 +232,10 @@
   <office:meta>
     <meta:creation-date>2017-10-20T23:41:04.964000000</meta:creation-date>
     <meta:generator>LibreOffice/7.0.6.2$Windows_X86_64 LibreOffice_project/144abb84a525d8e30c9dbbefa69cbbf2d8d4ae3b</meta:generator>
-    <dc:date>2021-09-16T20:12:58.243000000</dc:date>
-    <meta:editing-duration>PT43M4S</meta:editing-duration>
-    <meta:editing-cycles>24</meta:editing-cycles>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="22" meta:object-count="0"/>
+    <dc:date>2021-09-04T20:41:40.241000000</dc:date>
+    <meta:editing-duration>PT40M37S</meta:editing-duration>
+    <meta:editing-cycles>22</meta:editing-cycles>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="26" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -211,14 +247,14 @@
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaWidth" config:type="int">5445</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">19868</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">18965</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
               <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">43</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">2</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -443,9 +479,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2021-09-16">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2021-09-04">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="20:12:43.014000000">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="20:41:28.291000000">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>

<commit_message>
Getting categories and displaying them into select list in table.ejs so user can Select only those categories which are in database
</commit_message>
<xml_diff>
--- a/public/uploadedFile.xlsx
+++ b/public/uploadedFile.xlsx
@@ -54,71 +54,41 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>test1 test1</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>test2 test2</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>test3 test3</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>test4 test4</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>test5 test5</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>tarik besic</text:p>
           </table:table-cell>
           <table:table-cell/>
         </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>zijad zijic</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>
-              ensar 
-              <text:s/>
-              dzafo
-            </text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>
-              amar 
-              <text:s text:c="12"/>
-              silajdzic
-            </text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>
-              benjamin 
-              <text:s text:c="12"/>
-              salkic
-            </text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>abbas merdan</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>evvel kamenjas</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>hamza kamenjas</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>neko nekic</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1" table:number-rows-repeated="5">
+        <table:table-row table:style-name="ro1" table:number-rows-repeated="8">
           <table:table-cell table:number-columns-repeated="2"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
@@ -129,7 +99,37 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>lamija besic</text:p>
+            <text:p>ciko cikic</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>cikone cikone</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>caklone caklone</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>cako2 cako2</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>cako3 cako3</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>cako4 cako4</text:p>
           </table:table-cell>
           <table:table-cell/>
         </table:table-row>
@@ -139,55 +139,7 @@
           </table:table-cell>
           <table:table-cell/>
         </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>fadil masnopita</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>edis musanovic</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>zijad mehic</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>emin bucuk</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>emin keskic</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>adnan abdukic</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>adnan hadzic</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>amar hamzic</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1" table:number-rows-repeated="11">
+        <table:table-row table:style-name="ro1" table:number-rows-repeated="14">
           <table:table-cell table:number-columns-repeated="2"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
@@ -198,25 +150,37 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>friyer1 frizer 2</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>friyzer2 frizer 2</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>frizer3 frizer 3</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>frizer4 frizer4</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>frizer5 frizer5</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>malena iki</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>haris hadzic</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>amra amric</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>anesa anesic</text:p>
           </table:table-cell>
           <table:table-cell/>
         </table:table-row>
@@ -232,10 +196,10 @@
   <office:meta>
     <meta:creation-date>2017-10-20T23:41:04.964000000</meta:creation-date>
     <meta:generator>LibreOffice/7.0.6.2$Windows_X86_64 LibreOffice_project/144abb84a525d8e30c9dbbefa69cbbf2d8d4ae3b</meta:generator>
-    <dc:date>2021-09-04T20:41:40.241000000</dc:date>
-    <meta:editing-duration>PT40M37S</meta:editing-duration>
-    <meta:editing-cycles>22</meta:editing-cycles>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="26" meta:object-count="0"/>
+    <dc:date>2021-09-16T20:12:58.243000000</dc:date>
+    <meta:editing-duration>PT43M4S</meta:editing-duration>
+    <meta:editing-cycles>24</meta:editing-cycles>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="22" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -247,14 +211,14 @@
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaWidth" config:type="int">5445</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">18965</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">19868</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
               <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">2</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">43</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -479,9 +443,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2021-09-04">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2021-09-16">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="20:41:28.291000000">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="20:12:43.014000000">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>